<commit_message>
steps not calculating correctly
</commit_message>
<xml_diff>
--- a/lookup_table.xlsx
+++ b/lookup_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkh18\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkh18\ece350-newfinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A857A33-20C4-4238-B123-42155492DC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC846640-51EA-4C27-BCAC-E582C229CDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87B1DC4F-1B61-4B95-8E16-2F444BF00A72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Letter</t>
   </si>
@@ -150,16 +150,34 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>Pos*5</t>
+  </si>
+  <si>
+    <t>Prev</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,13 +203,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -209,16 +237,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{994B5B7C-BD0A-4F2A-9E48-9C032DB57E81}" name="Table1" displayName="Table1" ref="A1:E41" totalsRowShown="0">
-  <autoFilter ref="A1:E41" xr:uid="{994B5B7C-BD0A-4F2A-9E48-9C032DB57E81}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{994B5B7C-BD0A-4F2A-9E48-9C032DB57E81}" name="Table1" displayName="Table1" ref="A1:H41" totalsRowShown="0">
+  <autoFilter ref="A1:H41" xr:uid="{994B5B7C-BD0A-4F2A-9E48-9C032DB57E81}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H41">
+    <sortCondition ref="A1:A41"/>
+  </sortState>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D9695E8B-0420-4516-AE1B-351F74742A1B}" name="Letter"/>
     <tableColumn id="2" xr3:uid="{2CFF5F48-DDCF-4984-BCDC-5BBB9D0C119B}" name="Ascii (Hex)"/>
     <tableColumn id="3" xr3:uid="{6BE3E4C0-B2ED-47F2-BCEE-86C66F753732}" name="Scancode (1 indexed)"/>
     <tableColumn id="4" xr3:uid="{11038ECD-4244-4F73-AFBA-10C6ED4B7791}" name="Pos"/>
-    <tableColumn id="5" xr3:uid="{B3B5E0BA-E7A3-4E87-9C76-AB3029C29053}" name="Column1" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{A2AF51C2-6E5F-42BF-B1D2-DFAD0C003D29}" name="Pos*5" dataDxfId="0">
+      <calculatedColumnFormula>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B3B5E0BA-E7A3-4E87-9C76-AB3029C29053}" name="Column1" dataDxfId="3">
+      <calculatedColumnFormula>DEC2HEX(Table1[[#This Row],[Pos*5]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{570495E0-4690-4964-87DC-898D661BA966}" name="Prev" dataDxfId="2">
       <calculatedColumnFormula>DEC2HEX(Table1[[#This Row],[Pos]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" xr3:uid="{2761D85F-2240-4D4C-A9EC-4F2FA9B50159}" name="Column2" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -541,19 +579,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65659785-AC39-4611-BF99-147FC14CBE9A}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,694 +606,1072 @@
         <v>36</v>
       </c>
       <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>70</v>
+      </c>
+      <c r="D2">
+        <v>130</v>
+      </c>
+      <c r="E2">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>488</v>
+      </c>
+      <c r="F2" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>1E8</v>
+      </c>
+      <c r="G2" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>82</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B3">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>135</v>
+      </c>
+      <c r="E3">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>506</v>
+      </c>
+      <c r="F3" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>1FA</v>
+      </c>
+      <c r="G3" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>87</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>31</v>
+      </c>
+      <c r="D4">
+        <v>140</v>
+      </c>
+      <c r="E4">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>525</v>
+      </c>
+      <c r="F4" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>20D</v>
+      </c>
+      <c r="G4" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>8C</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>39</v>
+      </c>
+      <c r="D5">
+        <v>145</v>
+      </c>
+      <c r="E5">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>544</v>
+      </c>
+      <c r="F5" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>220</v>
+      </c>
+      <c r="G5" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>91</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>150</v>
+      </c>
+      <c r="E6">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>563</v>
+      </c>
+      <c r="F6" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>233</v>
+      </c>
+      <c r="G6" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>96</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>47</v>
+      </c>
+      <c r="D7">
+        <v>155</v>
+      </c>
+      <c r="E7">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>581</v>
+      </c>
+      <c r="F7" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>245</v>
+      </c>
+      <c r="G7" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>9B</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>160</v>
+      </c>
+      <c r="E8">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>600</v>
+      </c>
+      <c r="F8" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>258</v>
+      </c>
+      <c r="G8" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>A0</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>62</v>
+      </c>
+      <c r="D9">
+        <v>165</v>
+      </c>
+      <c r="E9">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>619</v>
+      </c>
+      <c r="F9" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>26B</v>
+      </c>
+      <c r="G9" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>A5</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>38</v>
+      </c>
+      <c r="C10">
+        <v>63</v>
+      </c>
+      <c r="D10">
+        <v>170</v>
+      </c>
+      <c r="E10">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>638</v>
+      </c>
+      <c r="F10" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>27E</v>
+      </c>
+      <c r="G10" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>AA</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>39</v>
+      </c>
+      <c r="C11">
+        <v>71</v>
+      </c>
+      <c r="D11">
+        <v>175</v>
+      </c>
+      <c r="E11">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>656</v>
+      </c>
+      <c r="F11" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>290</v>
+      </c>
+      <c r="G11" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>AF</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
         <v>41</v>
       </c>
-      <c r="C2">
+      <c r="C12">
         <v>29</v>
       </c>
-      <c r="D2">
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="E2" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+      <c r="E12">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F12" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>0</v>
+      </c>
+      <c r="G12" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B13">
         <v>42</v>
       </c>
-      <c r="C3">
+      <c r="C13">
         <v>51</v>
       </c>
-      <c r="D3">
+      <c r="D13">
         <v>5</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E13">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>19</v>
+      </c>
+      <c r="F13" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>13</v>
+      </c>
+      <c r="G13" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B14">
         <v>43</v>
       </c>
-      <c r="C4">
+      <c r="C14">
         <v>34</v>
       </c>
-      <c r="D4">
+      <c r="D14">
         <v>10</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E14">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>38</v>
+      </c>
+      <c r="F14" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>26</v>
+      </c>
+      <c r="G14" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>A</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B15">
         <v>44</v>
       </c>
-      <c r="C5">
+      <c r="C15">
         <v>36</v>
       </c>
-      <c r="D5">
+      <c r="D15">
         <v>15</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E15">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>56</v>
+      </c>
+      <c r="F15" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>38</v>
+      </c>
+      <c r="G15" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>F</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B16">
         <v>45</v>
       </c>
-      <c r="C6">
+      <c r="C16">
         <v>37</v>
       </c>
-      <c r="D6">
+      <c r="D16">
         <v>20</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E16">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>75</v>
+      </c>
+      <c r="F16" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>4B</v>
+      </c>
+      <c r="G16" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B17">
         <v>46</v>
       </c>
-      <c r="C7">
+      <c r="C17">
         <v>44</v>
       </c>
-      <c r="D7">
+      <c r="D17">
         <v>25</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E17">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>94</v>
+      </c>
+      <c r="F17" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>5E</v>
+      </c>
+      <c r="G17" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B18">
         <v>47</v>
       </c>
-      <c r="C8">
+      <c r="C18">
         <v>53</v>
       </c>
-      <c r="D8">
+      <c r="D18">
         <v>30</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E18">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>113</v>
+      </c>
+      <c r="F18" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>71</v>
+      </c>
+      <c r="G18" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>1E</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="H18" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B19">
         <v>48</v>
       </c>
-      <c r="C9">
+      <c r="C19">
         <v>52</v>
       </c>
-      <c r="D9">
+      <c r="D19">
         <v>35</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E19">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>131</v>
+      </c>
+      <c r="F19" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>83</v>
+      </c>
+      <c r="G19" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B20">
         <v>49</v>
       </c>
-      <c r="C10">
+      <c r="C20">
         <v>68</v>
       </c>
-      <c r="D10">
+      <c r="D20">
         <v>40</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E20">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>150</v>
+      </c>
+      <c r="F20" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>96</v>
+      </c>
+      <c r="G20" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="C11">
+      <c r="C21">
         <v>60</v>
       </c>
-      <c r="D11">
+      <c r="D21">
         <v>45</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E21">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>169</v>
+      </c>
+      <c r="F21" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>A9</v>
+      </c>
+      <c r="G21" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>2D</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C12">
+      <c r="C22">
         <v>67</v>
       </c>
-      <c r="D12">
+      <c r="D22">
         <v>50</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E22">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>188</v>
+      </c>
+      <c r="F22" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>BC</v>
+      </c>
+      <c r="G22" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B23" t="s">
         <v>29</v>
       </c>
-      <c r="C13">
+      <c r="C23">
         <v>76</v>
       </c>
-      <c r="D13">
+      <c r="D23">
         <v>55</v>
       </c>
-      <c r="E13" t="str">
+      <c r="E23">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>206</v>
+      </c>
+      <c r="F23" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>CE</v>
+      </c>
+      <c r="G23" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="H23" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="C14">
+      <c r="C24">
         <v>59</v>
       </c>
-      <c r="D14">
+      <c r="D24">
         <v>60</v>
       </c>
-      <c r="E14" t="str">
+      <c r="E24">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>225</v>
+      </c>
+      <c r="F24" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>E1</v>
+      </c>
+      <c r="G24" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>3C</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C15">
+      <c r="C25">
         <v>50</v>
       </c>
-      <c r="D15">
+      <c r="D25">
         <v>65</v>
       </c>
-      <c r="E15" t="str">
+      <c r="E25">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>244</v>
+      </c>
+      <c r="F25" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>F4</v>
+      </c>
+      <c r="G25" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C16">
+      <c r="C26">
         <v>69</v>
       </c>
-      <c r="D16">
+      <c r="D26">
         <v>70</v>
       </c>
-      <c r="E16" t="str">
+      <c r="E26">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>263</v>
+      </c>
+      <c r="F26" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>107</v>
+      </c>
+      <c r="G26" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B27">
         <v>50</v>
       </c>
-      <c r="C17">
+      <c r="C27">
         <v>78</v>
       </c>
-      <c r="D17">
+      <c r="D27">
         <v>75</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E27">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>281</v>
+      </c>
+      <c r="F27" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>119</v>
+      </c>
+      <c r="G27" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>4B</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B28">
         <v>51</v>
       </c>
-      <c r="C18">
+      <c r="C28">
         <v>22</v>
       </c>
-      <c r="D18">
+      <c r="D28">
         <v>80</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E28">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>300</v>
+      </c>
+      <c r="F28" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>12C</v>
+      </c>
+      <c r="G28" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="H28" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B29">
         <v>52</v>
       </c>
-      <c r="C19">
+      <c r="C29">
         <v>46</v>
       </c>
-      <c r="D19">
+      <c r="D29">
         <v>85</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E29">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>319</v>
+      </c>
+      <c r="F29" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>13F</v>
+      </c>
+      <c r="G29" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B30">
         <v>53</v>
       </c>
-      <c r="C20">
+      <c r="C30">
         <v>28</v>
       </c>
-      <c r="D20">
+      <c r="D30">
         <v>90</v>
       </c>
-      <c r="E20" t="str">
+      <c r="E30">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>338</v>
+      </c>
+      <c r="F30" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>152</v>
+      </c>
+      <c r="G30" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>5A</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B31">
         <v>54</v>
       </c>
-      <c r="C21">
+      <c r="C31">
         <v>45</v>
       </c>
-      <c r="D21">
+      <c r="D31">
         <v>95</v>
       </c>
-      <c r="E21" t="str">
+      <c r="E31">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>356</v>
+      </c>
+      <c r="F31" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>164</v>
+      </c>
+      <c r="G31" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>5F</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B32">
         <v>55</v>
       </c>
-      <c r="C22">
+      <c r="C32">
         <v>61</v>
       </c>
-      <c r="D22">
+      <c r="D32">
         <v>100</v>
       </c>
-      <c r="E22" t="str">
+      <c r="E32">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>375</v>
+      </c>
+      <c r="F32" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>177</v>
+      </c>
+      <c r="G32" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B33">
         <v>56</v>
       </c>
-      <c r="C23">
+      <c r="C33">
         <v>43</v>
       </c>
-      <c r="D23">
+      <c r="D33">
         <v>105</v>
       </c>
-      <c r="E23" t="str">
+      <c r="E33">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>394</v>
+      </c>
+      <c r="F33" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>18A</v>
+      </c>
+      <c r="G33" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="H33" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B34">
         <v>57</v>
       </c>
-      <c r="C24">
+      <c r="C34">
         <v>30</v>
       </c>
-      <c r="D24">
+      <c r="D34">
         <v>110</v>
       </c>
-      <c r="E24" t="str">
+      <c r="E34">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>413</v>
+      </c>
+      <c r="F34" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>19D</v>
+      </c>
+      <c r="G34" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>6E</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B35">
         <v>58</v>
       </c>
-      <c r="C25">
+      <c r="C35">
         <v>35</v>
       </c>
-      <c r="D25">
+      <c r="D35">
         <v>115</v>
       </c>
-      <c r="E25" t="str">
+      <c r="E35">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>431</v>
+      </c>
+      <c r="F35" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>1AF</v>
+      </c>
+      <c r="G35" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B36">
         <v>59</v>
       </c>
-      <c r="C26">
+      <c r="C36">
         <v>54</v>
       </c>
-      <c r="D26">
+      <c r="D36">
         <v>120</v>
       </c>
-      <c r="E26" t="str">
+      <c r="E36">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>450</v>
+      </c>
+      <c r="F36" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>1C2</v>
+      </c>
+      <c r="G36" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B37" t="s">
         <v>33</v>
       </c>
-      <c r="C27">
+      <c r="C37">
         <v>27</v>
       </c>
-      <c r="D27">
+      <c r="D37">
         <v>125</v>
       </c>
-      <c r="E27" t="str">
+      <c r="E37">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>469</v>
+      </c>
+      <c r="F37" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>1D5</v>
+      </c>
+      <c r="G37" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>7D</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28">
-        <v>30</v>
-      </c>
-      <c r="C28">
-        <v>70</v>
-      </c>
-      <c r="D28">
-        <v>130</v>
-      </c>
-      <c r="E28" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <v>31</v>
-      </c>
-      <c r="C29">
-        <v>23</v>
-      </c>
-      <c r="D29">
-        <v>135</v>
-      </c>
-      <c r="E29" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="B30">
-        <v>32</v>
-      </c>
-      <c r="C30">
-        <v>31</v>
-      </c>
-      <c r="D30">
-        <v>140</v>
-      </c>
-      <c r="E30" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>8C</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31">
-        <v>33</v>
-      </c>
-      <c r="C31">
-        <v>39</v>
-      </c>
-      <c r="D31">
-        <v>145</v>
-      </c>
-      <c r="E31" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>4</v>
-      </c>
-      <c r="B32">
-        <v>34</v>
-      </c>
-      <c r="C32">
-        <v>38</v>
-      </c>
-      <c r="D32">
-        <v>150</v>
-      </c>
-      <c r="E32" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>5</v>
-      </c>
-      <c r="B33">
-        <v>35</v>
-      </c>
-      <c r="C33">
-        <v>47</v>
-      </c>
-      <c r="D33">
-        <v>155</v>
-      </c>
-      <c r="E33" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>9B</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>6</v>
-      </c>
-      <c r="B34">
-        <v>36</v>
-      </c>
-      <c r="C34">
-        <v>55</v>
-      </c>
-      <c r="D34">
-        <v>160</v>
-      </c>
-      <c r="E34" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>A0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>7</v>
-      </c>
-      <c r="B35">
-        <v>37</v>
-      </c>
-      <c r="C35">
-        <v>62</v>
-      </c>
-      <c r="D35">
-        <v>165</v>
-      </c>
-      <c r="E35" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>A5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>8</v>
-      </c>
-      <c r="B36">
-        <v>38</v>
-      </c>
-      <c r="C36">
-        <v>63</v>
-      </c>
-      <c r="D36">
-        <v>170</v>
-      </c>
-      <c r="E36" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>AA</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>9</v>
-      </c>
-      <c r="B37">
-        <v>39</v>
-      </c>
-      <c r="C37">
-        <v>71</v>
-      </c>
-      <c r="D37">
-        <v>175</v>
-      </c>
-      <c r="E37" t="str">
-        <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>AF</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>180</v>
       </c>
-      <c r="E38" t="str">
+      <c r="E38">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>675</v>
+      </c>
+      <c r="F38" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>2A3</v>
+      </c>
+      <c r="G38" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>B4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>185</v>
       </c>
-      <c r="E39" t="str">
+      <c r="E39">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>694</v>
+      </c>
+      <c r="F39" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>2B6</v>
+      </c>
+      <c r="G39" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>B9</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>190</v>
       </c>
-      <c r="E40" t="str">
+      <c r="E40">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>713</v>
+      </c>
+      <c r="F40" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>2C9</v>
+      </c>
+      <c r="G40" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>BE</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>195</v>
       </c>
-      <c r="E41" t="str">
+      <c r="E41">
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
+        <v>731</v>
+      </c>
+      <c r="F41" t="str">
+        <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
+        <v>2DB</v>
+      </c>
+      <c r="G41" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>C3</v>
       </c>
+      <c r="H41" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Got three Steppers working, passing of pc to roxanna, next step is integrating new hall effect sensor
</commit_message>
<xml_diff>
--- a/lookup_table.xlsx
+++ b/lookup_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkh18\ece350-newfinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A39943-D074-4733-94F4-15B0FC86E8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FADA423-F0FE-4F97-8972-E8C8EE05A580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15330" yWindow="0" windowWidth="13470" windowHeight="15600" xr2:uid="{87B1DC4F-1B61-4B95-8E16-2F444BF00A72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87B1DC4F-1B61-4B95-8E16-2F444BF00A72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Letter</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>Prev</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Column2</t>
@@ -255,7 +252,9 @@
     <tableColumn id="8" xr3:uid="{570495E0-4690-4964-87DC-898D661BA966}" name="Prev" dataDxfId="1">
       <calculatedColumnFormula>DEC2HEX(Table1[[#This Row],[Pos]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{2761D85F-2240-4D4C-A9EC-4F2FA9B50159}" name="Column2" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{2761D85F-2240-4D4C-A9EC-4F2FA9B50159}" name="Column2" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Pos*5]]-E3</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -580,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65659785-AC39-4611-BF99-147FC14CBE9A}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -614,7 +613,7 @@
         <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -642,6 +641,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>82</v>
       </c>
+      <c r="H2">
+        <f>Table1[[#This Row],[Pos*5]]-E3</f>
+        <v>-18</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
@@ -668,6 +671,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>87</v>
       </c>
+      <c r="H3">
+        <f>Table1[[#This Row],[Pos*5]]-E4</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
@@ -694,6 +701,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>8C</v>
       </c>
+      <c r="H4">
+        <f>Table1[[#This Row],[Pos*5]]-E5</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
@@ -720,6 +731,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>91</v>
       </c>
+      <c r="H5">
+        <f>Table1[[#This Row],[Pos*5]]-E6</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
@@ -746,6 +761,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>96</v>
       </c>
+      <c r="H6">
+        <f>Table1[[#This Row],[Pos*5]]-E7</f>
+        <v>-18</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
@@ -772,6 +791,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>9B</v>
       </c>
+      <c r="H7">
+        <f>Table1[[#This Row],[Pos*5]]-E8</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
@@ -798,6 +821,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>A0</v>
       </c>
+      <c r="H8">
+        <f>Table1[[#This Row],[Pos*5]]-E9</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
@@ -824,6 +851,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>A5</v>
       </c>
+      <c r="H9">
+        <f>Table1[[#This Row],[Pos*5]]-E10</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
@@ -850,6 +881,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>AA</v>
       </c>
+      <c r="H10">
+        <f>Table1[[#This Row],[Pos*5]]-E11</f>
+        <v>-18</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
@@ -876,6 +911,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>AF</v>
       </c>
+      <c r="H11">
+        <f>Table1[[#This Row],[Pos*5]]-E12</f>
+        <v>656</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -902,6 +941,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>0</v>
       </c>
+      <c r="H12">
+        <f>Table1[[#This Row],[Pos*5]]-E13</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -928,6 +971,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>5</v>
       </c>
+      <c r="H13">
+        <f>Table1[[#This Row],[Pos*5]]-E14</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -954,6 +1001,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>A</v>
       </c>
+      <c r="H14">
+        <f>Table1[[#This Row],[Pos*5]]-E15</f>
+        <v>-18</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -980,6 +1031,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>F</v>
       </c>
+      <c r="H15">
+        <f>Table1[[#This Row],[Pos*5]]-E16</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -1006,6 +1061,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>14</v>
       </c>
+      <c r="H16">
+        <f>Table1[[#This Row],[Pos*5]]-E17</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -1032,6 +1091,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>19</v>
       </c>
+      <c r="H17">
+        <f>Table1[[#This Row],[Pos*5]]-E18</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
@@ -1058,8 +1121,9 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>1E</v>
       </c>
-      <c r="H18" t="s">
-        <v>40</v>
+      <c r="H18">
+        <f>Table1[[#This Row],[Pos*5]]-E19</f>
+        <v>-18</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1087,6 +1151,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>23</v>
       </c>
+      <c r="H19">
+        <f>Table1[[#This Row],[Pos*5]]-E20</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
@@ -1113,6 +1181,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>28</v>
       </c>
+      <c r="H20">
+        <f>Table1[[#This Row],[Pos*5]]-E21</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
@@ -1139,6 +1211,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>2D</v>
       </c>
+      <c r="H21">
+        <f>Table1[[#This Row],[Pos*5]]-E22</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
@@ -1165,6 +1241,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>32</v>
       </c>
+      <c r="H22">
+        <f>Table1[[#This Row],[Pos*5]]-E23</f>
+        <v>-18</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
@@ -1191,8 +1271,9 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>37</v>
       </c>
-      <c r="H23" t="s">
-        <v>40</v>
+      <c r="H23">
+        <f>Table1[[#This Row],[Pos*5]]-E24</f>
+        <v>-19</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1220,6 +1301,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>3C</v>
       </c>
+      <c r="H24">
+        <f>Table1[[#This Row],[Pos*5]]-E25</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
@@ -1246,6 +1331,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>41</v>
       </c>
+      <c r="H25">
+        <f>Table1[[#This Row],[Pos*5]]-E26</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
@@ -1272,6 +1361,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>46</v>
       </c>
+      <c r="H26">
+        <f>Table1[[#This Row],[Pos*5]]-E27</f>
+        <v>-18</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
@@ -1298,6 +1391,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>4B</v>
       </c>
+      <c r="H27">
+        <f>Table1[[#This Row],[Pos*5]]-E28</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
@@ -1324,8 +1421,9 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>50</v>
       </c>
-      <c r="H28" t="s">
-        <v>40</v>
+      <c r="H28">
+        <f>Table1[[#This Row],[Pos*5]]-E29</f>
+        <v>-19</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1353,6 +1451,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>55</v>
       </c>
+      <c r="H29">
+        <f>Table1[[#This Row],[Pos*5]]-E30</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
@@ -1379,6 +1481,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>5A</v>
       </c>
+      <c r="H30">
+        <f>Table1[[#This Row],[Pos*5]]-E31</f>
+        <v>-18</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
@@ -1405,6 +1511,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>5F</v>
       </c>
+      <c r="H31">
+        <f>Table1[[#This Row],[Pos*5]]-E32</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
@@ -1431,6 +1541,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>64</v>
       </c>
+      <c r="H32">
+        <f>Table1[[#This Row],[Pos*5]]-E33</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
@@ -1457,8 +1571,9 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>69</v>
       </c>
-      <c r="H33" t="s">
-        <v>40</v>
+      <c r="H33">
+        <f>Table1[[#This Row],[Pos*5]]-E34</f>
+        <v>-19</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1486,6 +1601,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>6E</v>
       </c>
+      <c r="H34">
+        <f>Table1[[#This Row],[Pos*5]]-E35</f>
+        <v>-18</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
@@ -1512,6 +1631,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>73</v>
       </c>
+      <c r="H35">
+        <f>Table1[[#This Row],[Pos*5]]-E36</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
@@ -1538,6 +1661,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>78</v>
       </c>
+      <c r="H36">
+        <f>Table1[[#This Row],[Pos*5]]-E37</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
@@ -1564,6 +1691,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>7D</v>
       </c>
+      <c r="H37">
+        <f>Table1[[#This Row],[Pos*5]]-E38</f>
+        <v>-206</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="D38">
@@ -1581,6 +1712,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>B4</v>
       </c>
+      <c r="H38">
+        <f>Table1[[#This Row],[Pos*5]]-E39</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="D39">
@@ -1598,6 +1733,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>B9</v>
       </c>
+      <c r="H39">
+        <f>Table1[[#This Row],[Pos*5]]-E40</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="D40">
@@ -1615,6 +1754,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>BE</v>
       </c>
+      <c r="H40">
+        <f>Table1[[#This Row],[Pos*5]]-E41</f>
+        <v>-18</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="D41">
@@ -1632,6 +1775,10 @@
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>C3</v>
       </c>
+      <c r="H41">
+        <f>Table1[[#This Row],[Pos*5]]-E42</f>
+        <v>-19</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="D42">
@@ -1648,6 +1795,10 @@
       <c r="G42" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
         <v>C8</v>
+      </c>
+      <c r="H42">
+        <f>Table1[[#This Row],[Pos*5]]-E43</f>
+        <v>750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the problem where it skips b/c offset
</commit_message>
<xml_diff>
--- a/lookup_table.xlsx
+++ b/lookup_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkh18\ece350-newfinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FADA423-F0FE-4F97-8972-E8C8EE05A580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935F5097-979A-4ADB-9CC3-69B7BBDA3908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87B1DC4F-1B61-4B95-8E16-2F444BF00A72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10230" windowHeight="15600" xr2:uid="{87B1DC4F-1B61-4B95-8E16-2F444BF00A72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,16 +243,16 @@
     <tableColumn id="2" xr3:uid="{2CFF5F48-DDCF-4984-BCDC-5BBB9D0C119B}" name="Ascii (Hex)"/>
     <tableColumn id="3" xr3:uid="{6BE3E4C0-B2ED-47F2-BCEE-86C66F753732}" name="Scancode (1 indexed)"/>
     <tableColumn id="4" xr3:uid="{11038ECD-4244-4F73-AFBA-10C6ED4B7791}" name="Pos"/>
-    <tableColumn id="7" xr3:uid="{A2AF51C2-6E5F-42BF-B1D2-DFAD0C003D29}" name="Pos*5" dataDxfId="3">
-      <calculatedColumnFormula>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{A2AF51C2-6E5F-42BF-B1D2-DFAD0C003D29}" name="Pos*5" dataDxfId="0">
+      <calculatedColumnFormula>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B3B5E0BA-E7A3-4E87-9C76-AB3029C29053}" name="Column1" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{B3B5E0BA-E7A3-4E87-9C76-AB3029C29053}" name="Column1" dataDxfId="3">
       <calculatedColumnFormula>DEC2HEX(Table1[[#This Row],[Pos*5]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{570495E0-4690-4964-87DC-898D661BA966}" name="Prev" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{570495E0-4690-4964-87DC-898D661BA966}" name="Prev" dataDxfId="2">
       <calculatedColumnFormula>DEC2HEX(Table1[[#This Row],[Pos]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{2761D85F-2240-4D4C-A9EC-4F2FA9B50159}" name="Column2" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{2761D85F-2240-4D4C-A9EC-4F2FA9B50159}" name="Column2" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[Pos*5]]-E3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -579,18 +579,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65659785-AC39-4611-BF99-147FC14CBE9A}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +616,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -630,12 +630,12 @@
         <v>130</v>
       </c>
       <c r="E2">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>488</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>520</v>
       </c>
       <c r="F2" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1E8</v>
+        <v>208</v>
       </c>
       <c r="G2" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -643,10 +643,10 @@
       </c>
       <c r="H2">
         <f>Table1[[#This Row],[Pos*5]]-E3</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -660,12 +660,12 @@
         <v>135</v>
       </c>
       <c r="E3">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>506</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>540</v>
       </c>
       <c r="F3" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1FA</v>
+        <v>21C</v>
       </c>
       <c r="G3" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -673,10 +673,10 @@
       </c>
       <c r="H3">
         <f>Table1[[#This Row],[Pos*5]]-E4</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -690,12 +690,12 @@
         <v>140</v>
       </c>
       <c r="E4">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>525</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>560</v>
       </c>
       <c r="F4" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>20D</v>
+        <v>230</v>
       </c>
       <c r="G4" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -703,10 +703,10 @@
       </c>
       <c r="H4">
         <f>Table1[[#This Row],[Pos*5]]-E5</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -720,12 +720,12 @@
         <v>145</v>
       </c>
       <c r="E5">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>544</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>580</v>
       </c>
       <c r="F5" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="G5" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -733,10 +733,10 @@
       </c>
       <c r="H5">
         <f>Table1[[#This Row],[Pos*5]]-E6</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -750,12 +750,12 @@
         <v>150</v>
       </c>
       <c r="E6">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>563</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>600</v>
       </c>
       <c r="F6" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="G6" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -763,10 +763,10 @@
       </c>
       <c r="H6">
         <f>Table1[[#This Row],[Pos*5]]-E7</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -780,12 +780,12 @@
         <v>155</v>
       </c>
       <c r="E7">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>581</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>620</v>
       </c>
       <c r="F7" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>245</v>
+        <v>26C</v>
       </c>
       <c r="G7" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -793,10 +793,10 @@
       </c>
       <c r="H7">
         <f>Table1[[#This Row],[Pos*5]]-E8</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -810,12 +810,12 @@
         <v>160</v>
       </c>
       <c r="E8">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>600</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>640</v>
       </c>
       <c r="F8" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="G8" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -823,10 +823,10 @@
       </c>
       <c r="H8">
         <f>Table1[[#This Row],[Pos*5]]-E9</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -840,12 +840,12 @@
         <v>165</v>
       </c>
       <c r="E9">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>619</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>660</v>
       </c>
       <c r="F9" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>26B</v>
+        <v>294</v>
       </c>
       <c r="G9" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -853,10 +853,10 @@
       </c>
       <c r="H9">
         <f>Table1[[#This Row],[Pos*5]]-E10</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -870,12 +870,12 @@
         <v>170</v>
       </c>
       <c r="E10">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>638</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>680</v>
       </c>
       <c r="F10" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>27E</v>
+        <v>2A8</v>
       </c>
       <c r="G10" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -883,10 +883,10 @@
       </c>
       <c r="H10">
         <f>Table1[[#This Row],[Pos*5]]-E11</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -900,12 +900,12 @@
         <v>175</v>
       </c>
       <c r="E11">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>656</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>700</v>
       </c>
       <c r="F11" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>290</v>
+        <v>2BC</v>
       </c>
       <c r="G11" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -913,10 +913,10 @@
       </c>
       <c r="H11">
         <f>Table1[[#This Row],[Pos*5]]-E12</f>
-        <v>656</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5),0)</f>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>0</v>
       </c>
       <c r="F12" t="str">
@@ -943,10 +943,10 @@
       </c>
       <c r="H12">
         <f>Table1[[#This Row],[Pos*5]]-E13</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -960,12 +960,12 @@
         <v>5</v>
       </c>
       <c r="E13">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>19</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>20</v>
       </c>
       <c r="F13" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -973,10 +973,10 @@
       </c>
       <c r="H13">
         <f>Table1[[#This Row],[Pos*5]]-E14</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -990,12 +990,12 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>38</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>40</v>
       </c>
       <c r="F14" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G14" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1003,10 +1003,10 @@
       </c>
       <c r="H14">
         <f>Table1[[#This Row],[Pos*5]]-E15</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1020,12 +1020,12 @@
         <v>15</v>
       </c>
       <c r="E15">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>56</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>60</v>
       </c>
       <c r="F15" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>38</v>
+        <v>3C</v>
       </c>
       <c r="G15" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1033,10 +1033,10 @@
       </c>
       <c r="H15">
         <f>Table1[[#This Row],[Pos*5]]-E16</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1050,12 +1050,12 @@
         <v>20</v>
       </c>
       <c r="E16">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>75</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>80</v>
       </c>
       <c r="F16" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>4B</v>
+        <v>50</v>
       </c>
       <c r="G16" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1063,10 +1063,10 @@
       </c>
       <c r="H16">
         <f>Table1[[#This Row],[Pos*5]]-E17</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1080,12 +1080,12 @@
         <v>25</v>
       </c>
       <c r="E17">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>94</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>100</v>
       </c>
       <c r="F17" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>5E</v>
+        <v>64</v>
       </c>
       <c r="G17" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1093,10 +1093,10 @@
       </c>
       <c r="H17">
         <f>Table1[[#This Row],[Pos*5]]-E18</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1110,12 +1110,12 @@
         <v>30</v>
       </c>
       <c r="E18">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>113</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>120</v>
       </c>
       <c r="F18" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G18" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1123,10 +1123,10 @@
       </c>
       <c r="H18">
         <f>Table1[[#This Row],[Pos*5]]-E19</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1140,12 +1140,12 @@
         <v>35</v>
       </c>
       <c r="E19">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>131</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>140</v>
       </c>
       <c r="F19" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>83</v>
+        <v>8C</v>
       </c>
       <c r="G19" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1153,10 +1153,10 @@
       </c>
       <c r="H19">
         <f>Table1[[#This Row],[Pos*5]]-E20</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1170,12 +1170,12 @@
         <v>40</v>
       </c>
       <c r="E20">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>150</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>160</v>
       </c>
       <c r="F20" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>96</v>
+        <v>A0</v>
       </c>
       <c r="G20" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1183,10 +1183,10 @@
       </c>
       <c r="H20">
         <f>Table1[[#This Row],[Pos*5]]-E21</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1200,12 +1200,12 @@
         <v>45</v>
       </c>
       <c r="E21">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>169</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>180</v>
       </c>
       <c r="F21" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>A9</v>
+        <v>B4</v>
       </c>
       <c r="G21" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1213,10 +1213,10 @@
       </c>
       <c r="H21">
         <f>Table1[[#This Row],[Pos*5]]-E22</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1230,12 +1230,12 @@
         <v>50</v>
       </c>
       <c r="E22">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>188</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>200</v>
       </c>
       <c r="F22" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>BC</v>
+        <v>C8</v>
       </c>
       <c r="G22" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1243,10 +1243,10 @@
       </c>
       <c r="H22">
         <f>Table1[[#This Row],[Pos*5]]-E23</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1260,12 +1260,12 @@
         <v>55</v>
       </c>
       <c r="E23">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>206</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>220</v>
       </c>
       <c r="F23" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>CE</v>
+        <v>DC</v>
       </c>
       <c r="G23" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1273,10 +1273,10 @@
       </c>
       <c r="H23">
         <f>Table1[[#This Row],[Pos*5]]-E24</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1290,12 +1290,12 @@
         <v>60</v>
       </c>
       <c r="E24">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>225</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>240</v>
       </c>
       <c r="F24" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>E1</v>
+        <v>F0</v>
       </c>
       <c r="G24" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1303,10 +1303,10 @@
       </c>
       <c r="H24">
         <f>Table1[[#This Row],[Pos*5]]-E25</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1320,12 +1320,12 @@
         <v>65</v>
       </c>
       <c r="E25">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>244</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>260</v>
       </c>
       <c r="F25" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>F4</v>
+        <v>104</v>
       </c>
       <c r="G25" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1333,10 +1333,10 @@
       </c>
       <c r="H25">
         <f>Table1[[#This Row],[Pos*5]]-E26</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1350,12 +1350,12 @@
         <v>70</v>
       </c>
       <c r="E26">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>263</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>280</v>
       </c>
       <c r="F26" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="G26" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1363,10 +1363,10 @@
       </c>
       <c r="H26">
         <f>Table1[[#This Row],[Pos*5]]-E27</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1380,12 +1380,12 @@
         <v>75</v>
       </c>
       <c r="E27">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>281</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>300</v>
       </c>
       <c r="F27" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>119</v>
+        <v>12C</v>
       </c>
       <c r="G27" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1393,10 +1393,10 @@
       </c>
       <c r="H27">
         <f>Table1[[#This Row],[Pos*5]]-E28</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1410,12 +1410,12 @@
         <v>80</v>
       </c>
       <c r="E28">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>300</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>320</v>
       </c>
       <c r="F28" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>12C</v>
+        <v>140</v>
       </c>
       <c r="G28" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1423,10 +1423,10 @@
       </c>
       <c r="H28">
         <f>Table1[[#This Row],[Pos*5]]-E29</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1440,12 +1440,12 @@
         <v>85</v>
       </c>
       <c r="E29">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>319</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>340</v>
       </c>
       <c r="F29" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>13F</v>
+        <v>154</v>
       </c>
       <c r="G29" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1453,10 +1453,10 @@
       </c>
       <c r="H29">
         <f>Table1[[#This Row],[Pos*5]]-E30</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1470,12 +1470,12 @@
         <v>90</v>
       </c>
       <c r="E30">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>338</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>360</v>
       </c>
       <c r="F30" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="G30" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1483,10 +1483,10 @@
       </c>
       <c r="H30">
         <f>Table1[[#This Row],[Pos*5]]-E31</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1500,12 +1500,12 @@
         <v>95</v>
       </c>
       <c r="E31">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>356</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>380</v>
       </c>
       <c r="F31" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>164</v>
+        <v>17C</v>
       </c>
       <c r="G31" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1513,10 +1513,10 @@
       </c>
       <c r="H31">
         <f>Table1[[#This Row],[Pos*5]]-E32</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -1530,12 +1530,12 @@
         <v>100</v>
       </c>
       <c r="E32">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>375</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>400</v>
       </c>
       <c r="F32" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="G32" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1543,10 +1543,10 @@
       </c>
       <c r="H32">
         <f>Table1[[#This Row],[Pos*5]]-E33</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1560,12 +1560,12 @@
         <v>105</v>
       </c>
       <c r="E33">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>394</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>420</v>
       </c>
       <c r="F33" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>18A</v>
+        <v>1A4</v>
       </c>
       <c r="G33" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1573,10 +1573,10 @@
       </c>
       <c r="H33">
         <f>Table1[[#This Row],[Pos*5]]-E34</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1590,12 +1590,12 @@
         <v>110</v>
       </c>
       <c r="E34">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>413</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>440</v>
       </c>
       <c r="F34" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>19D</v>
+        <v>1B8</v>
       </c>
       <c r="G34" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1603,10 +1603,10 @@
       </c>
       <c r="H34">
         <f>Table1[[#This Row],[Pos*5]]-E35</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -1620,12 +1620,12 @@
         <v>115</v>
       </c>
       <c r="E35">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>431</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>460</v>
       </c>
       <c r="F35" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1AF</v>
+        <v>1CC</v>
       </c>
       <c r="G35" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1633,10 +1633,10 @@
       </c>
       <c r="H35">
         <f>Table1[[#This Row],[Pos*5]]-E36</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -1650,12 +1650,12 @@
         <v>120</v>
       </c>
       <c r="E36">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>450</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>480</v>
       </c>
       <c r="F36" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1C2</v>
+        <v>1E0</v>
       </c>
       <c r="G36" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1663,10 +1663,10 @@
       </c>
       <c r="H36">
         <f>Table1[[#This Row],[Pos*5]]-E37</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -1680,12 +1680,12 @@
         <v>125</v>
       </c>
       <c r="E37">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>469</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>500</v>
       </c>
       <c r="F37" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1D5</v>
+        <v>1F4</v>
       </c>
       <c r="G37" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1693,20 +1693,20 @@
       </c>
       <c r="H37">
         <f>Table1[[#This Row],[Pos*5]]-E38</f>
-        <v>-206</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>-220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>180</v>
       </c>
       <c r="E38">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>675</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>720</v>
       </c>
       <c r="F38" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>2A3</v>
+        <v>2D0</v>
       </c>
       <c r="G38" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1714,20 +1714,20 @@
       </c>
       <c r="H38">
         <f>Table1[[#This Row],[Pos*5]]-E39</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>185</v>
       </c>
       <c r="E39">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>694</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>740</v>
       </c>
       <c r="F39" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>2B6</v>
+        <v>2E4</v>
       </c>
       <c r="G39" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1735,20 +1735,20 @@
       </c>
       <c r="H39">
         <f>Table1[[#This Row],[Pos*5]]-E40</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>190</v>
       </c>
       <c r="E40">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>713</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>760</v>
       </c>
       <c r="F40" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>2C9</v>
+        <v>2F8</v>
       </c>
       <c r="G40" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1756,20 +1756,20 @@
       </c>
       <c r="H40">
         <f>Table1[[#This Row],[Pos*5]]-E41</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>195</v>
       </c>
       <c r="E41">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>731</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>780</v>
       </c>
       <c r="F41" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>2DB</v>
+        <v>30C</v>
       </c>
       <c r="G41" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1777,20 +1777,20 @@
       </c>
       <c r="H41">
         <f>Table1[[#This Row],[Pos*5]]-E42</f>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D42">
         <v>200</v>
       </c>
       <c r="E42">
-        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/4),0)</f>
-        <v>750</v>
+        <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
+        <v>800</v>
       </c>
       <c r="F42" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>2EE</v>
+        <v>320</v>
       </c>
       <c r="G42" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="H42">
         <f>Table1[[#This Row],[Pos*5]]-E43</f>
-        <v>750</v>
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Saving before I try a new animation
</commit_message>
<xml_diff>
--- a/lookup_table.xlsx
+++ b/lookup_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkh18\ece350-newfinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935F5097-979A-4ADB-9CC3-69B7BBDA3908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059DF362-BA42-498C-8945-A8A7B44EA931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10230" windowHeight="15600" xr2:uid="{87B1DC4F-1B61-4B95-8E16-2F444BF00A72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Letter</t>
   </si>
@@ -159,13 +159,25 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,13 +191,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -197,13 +227,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -243,16 +277,16 @@
     <tableColumn id="2" xr3:uid="{2CFF5F48-DDCF-4984-BCDC-5BBB9D0C119B}" name="Ascii (Hex)"/>
     <tableColumn id="3" xr3:uid="{6BE3E4C0-B2ED-47F2-BCEE-86C66F753732}" name="Scancode (1 indexed)"/>
     <tableColumn id="4" xr3:uid="{11038ECD-4244-4F73-AFBA-10C6ED4B7791}" name="Pos"/>
-    <tableColumn id="7" xr3:uid="{A2AF51C2-6E5F-42BF-B1D2-DFAD0C003D29}" name="Pos*5" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{A2AF51C2-6E5F-42BF-B1D2-DFAD0C003D29}" name="Pos*5" dataDxfId="3" dataCellStyle="Good">
       <calculatedColumnFormula>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B3B5E0BA-E7A3-4E87-9C76-AB3029C29053}" name="Column1" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{B3B5E0BA-E7A3-4E87-9C76-AB3029C29053}" name="Column1" dataDxfId="2">
       <calculatedColumnFormula>DEC2HEX(Table1[[#This Row],[Pos*5]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{570495E0-4690-4964-87DC-898D661BA966}" name="Prev" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{570495E0-4690-4964-87DC-898D661BA966}" name="Prev" dataDxfId="1">
       <calculatedColumnFormula>DEC2HEX(Table1[[#This Row],[Pos]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{2761D85F-2240-4D4C-A9EC-4F2FA9B50159}" name="Column2" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{2761D85F-2240-4D4C-A9EC-4F2FA9B50159}" name="Column2" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[Pos*5]]-E3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -579,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65659785-AC39-4611-BF99-147FC14CBE9A}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +663,7 @@
       <c r="D2">
         <v>130</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>520</v>
       </c>
@@ -659,7 +693,7 @@
       <c r="D3">
         <v>135</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>540</v>
       </c>
@@ -689,7 +723,7 @@
       <c r="D4">
         <v>140</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>560</v>
       </c>
@@ -719,7 +753,7 @@
       <c r="D5">
         <v>145</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>580</v>
       </c>
@@ -749,7 +783,7 @@
       <c r="D6">
         <v>150</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>600</v>
       </c>
@@ -779,7 +813,7 @@
       <c r="D7">
         <v>155</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>620</v>
       </c>
@@ -809,7 +843,7 @@
       <c r="D8">
         <v>160</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>640</v>
       </c>
@@ -839,7 +873,7 @@
       <c r="D9">
         <v>165</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>660</v>
       </c>
@@ -869,7 +903,7 @@
       <c r="D10">
         <v>170</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>680</v>
       </c>
@@ -899,7 +933,7 @@
       <c r="D11">
         <v>175</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>700</v>
       </c>
@@ -929,7 +963,7 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>0</v>
       </c>
@@ -959,7 +993,7 @@
       <c r="D13">
         <v>5</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>20</v>
       </c>
@@ -989,7 +1023,7 @@
       <c r="D14">
         <v>10</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>40</v>
       </c>
@@ -1019,7 +1053,7 @@
       <c r="D15">
         <v>15</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>60</v>
       </c>
@@ -1049,7 +1083,7 @@
       <c r="D16">
         <v>20</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>80</v>
       </c>
@@ -1079,7 +1113,7 @@
       <c r="D17">
         <v>25</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>100</v>
       </c>
@@ -1109,7 +1143,7 @@
       <c r="D18">
         <v>30</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>120</v>
       </c>
@@ -1139,7 +1173,7 @@
       <c r="D19">
         <v>35</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>140</v>
       </c>
@@ -1169,7 +1203,7 @@
       <c r="D20">
         <v>40</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>160</v>
       </c>
@@ -1199,7 +1233,7 @@
       <c r="D21">
         <v>45</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>180</v>
       </c>
@@ -1229,7 +1263,7 @@
       <c r="D22">
         <v>50</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>200</v>
       </c>
@@ -1259,7 +1293,7 @@
       <c r="D23">
         <v>55</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>220</v>
       </c>
@@ -1289,7 +1323,7 @@
       <c r="D24">
         <v>60</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>240</v>
       </c>
@@ -1319,7 +1353,7 @@
       <c r="D25">
         <v>65</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>260</v>
       </c>
@@ -1349,7 +1383,7 @@
       <c r="D26">
         <v>70</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>280</v>
       </c>
@@ -1379,7 +1413,7 @@
       <c r="D27">
         <v>75</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>300</v>
       </c>
@@ -1409,7 +1443,7 @@
       <c r="D28">
         <v>80</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>320</v>
       </c>
@@ -1439,7 +1473,7 @@
       <c r="D29">
         <v>85</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>340</v>
       </c>
@@ -1469,7 +1503,7 @@
       <c r="D30">
         <v>90</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>360</v>
       </c>
@@ -1499,7 +1533,7 @@
       <c r="D31">
         <v>95</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>380</v>
       </c>
@@ -1529,7 +1563,7 @@
       <c r="D32">
         <v>100</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>400</v>
       </c>
@@ -1559,7 +1593,7 @@
       <c r="D33">
         <v>105</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>420</v>
       </c>
@@ -1589,7 +1623,7 @@
       <c r="D34">
         <v>110</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>440</v>
       </c>
@@ -1619,7 +1653,7 @@
       <c r="D35">
         <v>115</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>460</v>
       </c>
@@ -1649,7 +1683,7 @@
       <c r="D36">
         <v>120</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>480</v>
       </c>
@@ -1679,7 +1713,7 @@
       <c r="D37">
         <v>125</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>500</v>
       </c>
@@ -1697,10 +1731,16 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
       <c r="D38">
         <v>180</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>720</v>
       </c>
@@ -1718,10 +1758,16 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
       <c r="D39">
         <v>185</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>740</v>
       </c>
@@ -1739,10 +1785,16 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40">
+        <v>77</v>
+      </c>
       <c r="D40">
         <v>190</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>760</v>
       </c>
@@ -1760,10 +1812,19 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="2">
+        <v>32</v>
+      </c>
+      <c r="C41">
+        <v>42</v>
+      </c>
       <c r="D41">
         <v>195</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>780</v>
       </c>
@@ -1784,7 +1845,7 @@
       <c r="D42">
         <v>200</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
         <v>800</v>
       </c>
@@ -1804,8 +1865,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
steppers 5 and 6 trying to move but not moving
</commit_message>
<xml_diff>
--- a/lookup_table.xlsx
+++ b/lookup_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkh18\ece350-newfinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059DF362-BA42-498C-8945-A8A7B44EA931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37953EE7-279C-4471-9E05-7F707E4FF9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10230" windowHeight="15600" xr2:uid="{87B1DC4F-1B61-4B95-8E16-2F444BF00A72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10230" windowHeight="14985" xr2:uid="{87B1DC4F-1B61-4B95-8E16-2F444BF00A72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -270,7 +270,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{994B5B7C-BD0A-4F2A-9E48-9C032DB57E81}" name="Table1" displayName="Table1" ref="A1:H42" totalsRowShown="0">
   <autoFilter ref="A1:H42" xr:uid="{994B5B7C-BD0A-4F2A-9E48-9C032DB57E81}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H42">
-    <sortCondition ref="A1:A42"/>
+    <sortCondition ref="E1:E42"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D9695E8B-0420-4516-AE1B-351F74742A1B}" name="Letter"/>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65659785-AC39-4611-BF99-147FC14CBE9A}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,29 +651,29 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>29</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-      <c r="C2">
-        <v>70</v>
-      </c>
-      <c r="D2">
-        <v>130</v>
-      </c>
       <c r="E2" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>520</v>
+        <v>0</v>
       </c>
       <c r="F2" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="G2" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <f>Table1[[#This Row],[Pos*5]]-E3</f>
@@ -681,29 +681,29 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C3">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D3">
-        <v>135</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>540</v>
+        <v>20</v>
       </c>
       <c r="F3" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>21C</v>
+        <v>14</v>
       </c>
       <c r="G3" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="H3">
         <f>Table1[[#This Row],[Pos*5]]-E4</f>
@@ -711,29 +711,29 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C4">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>560</v>
+        <v>40</v>
       </c>
       <c r="F4" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>230</v>
+        <v>28</v>
       </c>
       <c r="G4" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>8C</v>
+        <v>A</v>
       </c>
       <c r="H4">
         <f>Table1[[#This Row],[Pos*5]]-E5</f>
@@ -741,29 +741,29 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C5">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D5">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>580</v>
+        <v>60</v>
       </c>
       <c r="F5" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>244</v>
+        <v>3C</v>
       </c>
       <c r="G5" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>91</v>
+        <v>F</v>
       </c>
       <c r="H5">
         <f>Table1[[#This Row],[Pos*5]]-E6</f>
@@ -771,29 +771,29 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C6">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>600</v>
+        <v>80</v>
       </c>
       <c r="F6" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>258</v>
+        <v>50</v>
       </c>
       <c r="G6" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <f>Table1[[#This Row],[Pos*5]]-E7</f>
@@ -801,29 +801,29 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
+      <c r="A7" t="s">
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C7">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D7">
-        <v>155</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>620</v>
+        <v>100</v>
       </c>
       <c r="F7" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>26C</v>
+        <v>64</v>
       </c>
       <c r="G7" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>9B</v>
+        <v>19</v>
       </c>
       <c r="H7">
         <f>Table1[[#This Row],[Pos*5]]-E8</f>
@@ -831,29 +831,29 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
+      <c r="A8" t="s">
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C8">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8">
-        <v>160</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>640</v>
+        <v>120</v>
       </c>
       <c r="F8" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>280</v>
+        <v>78</v>
       </c>
       <c r="G8" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>A0</v>
+        <v>1E</v>
       </c>
       <c r="H8">
         <f>Table1[[#This Row],[Pos*5]]-E9</f>
@@ -861,29 +861,29 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C9">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D9">
-        <v>165</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>660</v>
+        <v>140</v>
       </c>
       <c r="F9" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>294</v>
+        <v>8C</v>
       </c>
       <c r="G9" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>A5</v>
+        <v>23</v>
       </c>
       <c r="H9">
         <f>Table1[[#This Row],[Pos*5]]-E10</f>
@@ -891,29 +891,29 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
+      <c r="A10" t="s">
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C10">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D10">
-        <v>170</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>680</v>
+        <v>160</v>
       </c>
       <c r="F10" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>2A8</v>
+        <v>A0</v>
       </c>
       <c r="G10" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>AA</v>
+        <v>28</v>
       </c>
       <c r="H10">
         <f>Table1[[#This Row],[Pos*5]]-E11</f>
@@ -921,59 +921,59 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>39</v>
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
       </c>
       <c r="C11">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D11">
-        <v>175</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>700</v>
+        <v>180</v>
       </c>
       <c r="F11" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>2BC</v>
+        <v>B4</v>
       </c>
       <c r="G11" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>AF</v>
+        <v>2D</v>
       </c>
       <c r="H11">
         <f>Table1[[#This Row],[Pos*5]]-E12</f>
-        <v>700</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <v>41</v>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
       </c>
       <c r="C12">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F12" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>0</v>
+        <v>C8</v>
       </c>
       <c r="G12" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H12">
         <f>Table1[[#This Row],[Pos*5]]-E13</f>
@@ -982,28 +982,28 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>42</v>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
       </c>
       <c r="C13">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="F13" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>14</v>
+        <v>DC</v>
       </c>
       <c r="G13" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="H13">
         <f>Table1[[#This Row],[Pos*5]]-E14</f>
@@ -1012,28 +1012,28 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14">
-        <v>43</v>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
       </c>
       <c r="C14">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>40</v>
+        <v>240</v>
       </c>
       <c r="F14" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>28</v>
+        <v>F0</v>
       </c>
       <c r="G14" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>A</v>
+        <v>3C</v>
       </c>
       <c r="H14">
         <f>Table1[[#This Row],[Pos*5]]-E15</f>
@@ -1042,28 +1042,28 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15">
-        <v>44</v>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
       </c>
       <c r="C15">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D15">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E15" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>60</v>
+        <v>260</v>
       </c>
       <c r="F15" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>3C</v>
+        <v>104</v>
       </c>
       <c r="G15" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>F</v>
+        <v>41</v>
       </c>
       <c r="H15">
         <f>Table1[[#This Row],[Pos*5]]-E16</f>
@@ -1072,28 +1072,28 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
       </c>
       <c r="C16">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="D16">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="E16" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="F16" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="G16" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="H16">
         <f>Table1[[#This Row],[Pos*5]]-E17</f>
@@ -1102,28 +1102,28 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C17">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E17" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F17" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>64</v>
+        <v>12C</v>
       </c>
       <c r="G17" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>19</v>
+        <v>4B</v>
       </c>
       <c r="H17">
         <f>Table1[[#This Row],[Pos*5]]-E18</f>
@@ -1132,28 +1132,28 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C18">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="E18" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>120</v>
+        <v>320</v>
       </c>
       <c r="F18" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="G18" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>1E</v>
+        <v>50</v>
       </c>
       <c r="H18">
         <f>Table1[[#This Row],[Pos*5]]-E19</f>
@@ -1162,28 +1162,28 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C19">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D19">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>140</v>
+        <v>340</v>
       </c>
       <c r="F19" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>8C</v>
+        <v>154</v>
       </c>
       <c r="G19" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="H19">
         <f>Table1[[#This Row],[Pos*5]]-E20</f>
@@ -1192,28 +1192,28 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C20">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="D20">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="E20" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="F20" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>A0</v>
+        <v>168</v>
       </c>
       <c r="G20" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>28</v>
+        <v>5A</v>
       </c>
       <c r="H20">
         <f>Table1[[#This Row],[Pos*5]]-E21</f>
@@ -1222,28 +1222,28 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>54</v>
       </c>
       <c r="C21">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D21">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="E21" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>180</v>
+        <v>380</v>
       </c>
       <c r="F21" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>B4</v>
+        <v>17C</v>
       </c>
       <c r="G21" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>2D</v>
+        <v>5F</v>
       </c>
       <c r="H21">
         <f>Table1[[#This Row],[Pos*5]]-E22</f>
@@ -1252,28 +1252,28 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>55</v>
       </c>
       <c r="C22">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D22">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E22" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F22" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>C8</v>
+        <v>190</v>
       </c>
       <c r="G22" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="H22">
         <f>Table1[[#This Row],[Pos*5]]-E23</f>
@@ -1282,28 +1282,28 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>56</v>
       </c>
       <c r="C23">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="D23">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="E23" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>220</v>
+        <v>420</v>
       </c>
       <c r="F23" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>DC</v>
+        <v>1A4</v>
       </c>
       <c r="G23" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="H23">
         <f>Table1[[#This Row],[Pos*5]]-E24</f>
@@ -1312,28 +1312,28 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>57</v>
+      </c>
+      <c r="C24">
         <v>30</v>
       </c>
-      <c r="C24">
-        <v>59</v>
-      </c>
       <c r="D24">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E24" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>240</v>
+        <v>440</v>
       </c>
       <c r="F24" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>F0</v>
+        <v>1B8</v>
       </c>
       <c r="G24" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>3C</v>
+        <v>6E</v>
       </c>
       <c r="H24">
         <f>Table1[[#This Row],[Pos*5]]-E25</f>
@@ -1342,28 +1342,28 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>58</v>
       </c>
       <c r="C25">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D25">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="E25" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>260</v>
+        <v>460</v>
       </c>
       <c r="F25" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>104</v>
+        <v>1CC</v>
       </c>
       <c r="G25" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="H25">
         <f>Table1[[#This Row],[Pos*5]]-E26</f>
@@ -1372,28 +1372,28 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>59</v>
       </c>
       <c r="C26">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D26">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="E26" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>280</v>
+        <v>480</v>
       </c>
       <c r="F26" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>118</v>
+        <v>1E0</v>
       </c>
       <c r="G26" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="H26">
         <f>Table1[[#This Row],[Pos*5]]-E27</f>
@@ -1402,28 +1402,28 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27">
-        <v>50</v>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
       </c>
       <c r="C27">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="D27">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="E27" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="F27" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>12C</v>
+        <v>1F4</v>
       </c>
       <c r="G27" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>4B</v>
+        <v>7D</v>
       </c>
       <c r="H27">
         <f>Table1[[#This Row],[Pos*5]]-E28</f>
@@ -1431,29 +1431,29 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>17</v>
+      <c r="A28">
+        <v>0</v>
       </c>
       <c r="B28">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C28">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="D28">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="E28" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>320</v>
+        <v>520</v>
       </c>
       <c r="F28" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>140</v>
+        <v>208</v>
       </c>
       <c r="G28" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="H28">
         <f>Table1[[#This Row],[Pos*5]]-E29</f>
@@ -1461,29 +1461,29 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>18</v>
+      <c r="A29">
+        <v>1</v>
       </c>
       <c r="B29">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C29">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="D29">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="E29" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>340</v>
+        <v>540</v>
       </c>
       <c r="F29" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>154</v>
+        <v>21C</v>
       </c>
       <c r="G29" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="H29">
         <f>Table1[[#This Row],[Pos*5]]-E30</f>
@@ -1491,29 +1491,29 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>19</v>
+      <c r="A30">
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C30">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D30">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="E30" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>360</v>
+        <v>560</v>
       </c>
       <c r="F30" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>168</v>
+        <v>230</v>
       </c>
       <c r="G30" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>5A</v>
+        <v>8C</v>
       </c>
       <c r="H30">
         <f>Table1[[#This Row],[Pos*5]]-E31</f>
@@ -1521,29 +1521,29 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>20</v>
+      <c r="A31">
+        <v>3</v>
       </c>
       <c r="B31">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C31">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D31">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="E31" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>380</v>
+        <v>580</v>
       </c>
       <c r="F31" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>17C</v>
+        <v>244</v>
       </c>
       <c r="G31" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>5F</v>
+        <v>91</v>
       </c>
       <c r="H31">
         <f>Table1[[#This Row],[Pos*5]]-E32</f>
@@ -1551,29 +1551,29 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>21</v>
+      <c r="A32">
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C32">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D32">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E32" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="F32" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>190</v>
+        <v>258</v>
       </c>
       <c r="G32" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="H32">
         <f>Table1[[#This Row],[Pos*5]]-E33</f>
@@ -1581,29 +1581,29 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>22</v>
+      <c r="A33">
+        <v>5</v>
       </c>
       <c r="B33">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C33">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D33">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="E33" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>420</v>
+        <v>620</v>
       </c>
       <c r="F33" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1A4</v>
+        <v>26C</v>
       </c>
       <c r="G33" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>69</v>
+        <v>9B</v>
       </c>
       <c r="H33">
         <f>Table1[[#This Row],[Pos*5]]-E34</f>
@@ -1611,29 +1611,29 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>23</v>
+      <c r="A34">
+        <v>6</v>
       </c>
       <c r="B34">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C34">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D34">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="E34" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>440</v>
+        <v>640</v>
       </c>
       <c r="F34" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1B8</v>
+        <v>280</v>
       </c>
       <c r="G34" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>6E</v>
+        <v>A0</v>
       </c>
       <c r="H34">
         <f>Table1[[#This Row],[Pos*5]]-E35</f>
@@ -1641,29 +1641,29 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>24</v>
+      <c r="A35">
+        <v>7</v>
       </c>
       <c r="B35">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C35">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="D35">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="E35" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>460</v>
+        <v>660</v>
       </c>
       <c r="F35" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1CC</v>
+        <v>294</v>
       </c>
       <c r="G35" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>73</v>
+        <v>A5</v>
       </c>
       <c r="H35">
         <f>Table1[[#This Row],[Pos*5]]-E36</f>
@@ -1671,29 +1671,29 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>25</v>
+      <c r="A36">
+        <v>8</v>
       </c>
       <c r="B36">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C36">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D36">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="E36" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>480</v>
+        <v>680</v>
       </c>
       <c r="F36" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1E0</v>
+        <v>2A8</v>
       </c>
       <c r="G36" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>78</v>
+        <v>AA</v>
       </c>
       <c r="H36">
         <f>Table1[[#This Row],[Pos*5]]-E37</f>
@@ -1701,33 +1701,33 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" t="s">
-        <v>33</v>
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>39</v>
       </c>
       <c r="C37">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="D37">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="E37" s="1">
         <f>ROUND(Table1[[#This Row],[Pos]]*(5-5/5),0)</f>
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="F37" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos*5]])</f>
-        <v>1F4</v>
+        <v>2BC</v>
       </c>
       <c r="G37" t="str">
         <f>DEC2HEX(Table1[[#This Row],[Pos]])</f>
-        <v>7D</v>
+        <v>AF</v>
       </c>
       <c r="H37">
         <f>Table1[[#This Row],[Pos*5]]-E38</f>
-        <v>-220</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>